<commit_message>
Update excel file and little cleanup of schematic
</commit_message>
<xml_diff>
--- a/Teensy Shield Arduino Headers Through Hole/TeensyduinoTH BOM v.1.xlsx
+++ b/Teensy Shield Arduino Headers Through Hole/TeensyduinoTH BOM v.1.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="14760" yWindow="-60" windowWidth="14685" windowHeight="12840"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Parts List" sheetId="1" r:id="rId1"/>
+    <sheet name="Parts Usage" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="diptrace_parts_list" localSheetId="0">Sheet1!#REF!</definedName>
-    <definedName name="diptrace_parts_list_1" localSheetId="0">Sheet1!$C$1:$I$19</definedName>
-    <definedName name="TeensyduinoTH_Parts_list" localSheetId="1">Sheet2!$A$1:$F$26</definedName>
+    <definedName name="diptrace_parts_list" localSheetId="0">'Parts List'!#REF!</definedName>
+    <definedName name="diptrace_parts_list_1" localSheetId="0">'Parts List'!$C$1:$I$19</definedName>
+    <definedName name="TeensyduinoTH_Parts_list" localSheetId="1">'Parts Usage'!$C$1:$E$32</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="156">
   <si>
     <t>Value</t>
   </si>
@@ -329,93 +329,27 @@
     <t>SWITCH TACT 6X3.5MM H=4.3MM 130G</t>
   </si>
   <si>
-    <t>BTN, RST</t>
-  </si>
-  <si>
-    <t>B3U-1000P</t>
-  </si>
-  <si>
-    <t>MOU506-FSCM</t>
-  </si>
-  <si>
     <t>C1, C2, C3, C5, C6, C7, C14</t>
   </si>
   <si>
     <t>CAP100</t>
   </si>
   <si>
-    <t>CAP-2.54/6.6x3</t>
-  </si>
-  <si>
     <t>C4, C8, C20</t>
   </si>
   <si>
     <t>1uf</t>
   </si>
   <si>
-    <t>CAP_POLPTH1</t>
-  </si>
-  <si>
-    <t>CAPPR-2.5/6.3h7</t>
-  </si>
-  <si>
-    <t>1N4130</t>
-  </si>
-  <si>
     <t>DO-35</t>
   </si>
   <si>
     <t>D2</t>
   </si>
   <si>
-    <t>DIODE-ZENERSMB</t>
-  </si>
-  <si>
-    <t>SOD323-W</t>
-  </si>
-  <si>
-    <t>5.1v</t>
-  </si>
-  <si>
-    <t>IOREF, JAX1, JAX2, JCN1, JCN2, JCN3, JCN4, JCN5, JCN6</t>
-  </si>
-  <si>
-    <t>HDR-1x3</t>
-  </si>
-  <si>
-    <t>OSTTC040162</t>
-  </si>
-  <si>
-    <t>TB-1x4/5/21x7.5/Sc_H</t>
-  </si>
-  <si>
-    <t>PPTC061LFBN-RC</t>
-  </si>
-  <si>
-    <t>HDRF-1x6T/2.54/16x3</t>
-  </si>
-  <si>
-    <t>PPTC081LFBN-RC</t>
-  </si>
-  <si>
-    <t>HDRF-1x8T/2.54/21x3</t>
-  </si>
-  <si>
-    <t>PPTC101LFBN-RC</t>
-  </si>
-  <si>
-    <t>HDRF-1x10T/2.54/26x3</t>
-  </si>
-  <si>
-    <t>LED, PWR</t>
-  </si>
-  <si>
     <t>LED3MM</t>
   </si>
   <si>
-    <t>2N3904</t>
-  </si>
-  <si>
     <t>RES400</t>
   </si>
   <si>
@@ -425,30 +359,12 @@
     <t>R4</t>
   </si>
   <si>
-    <t>R5, R7, R9</t>
-  </si>
-  <si>
     <t>MCP1700_TO</t>
   </si>
   <si>
-    <t>U2</t>
-  </si>
-  <si>
-    <t>AVR_SPI_PRG_6PTH</t>
-  </si>
-  <si>
-    <t>2X3</t>
-  </si>
-  <si>
-    <t>TEENSY_3.1_ALLPINS-MIN</t>
-  </si>
-  <si>
     <t>LM2940T5.0</t>
   </si>
   <si>
-    <t>TO-220</t>
-  </si>
-  <si>
     <t>TDK</t>
   </si>
   <si>
@@ -543,6 +459,78 @@
   </si>
   <si>
     <t>Fairchild</t>
+  </si>
+  <si>
+    <t>C4, C8</t>
+  </si>
+  <si>
+    <t>O - Voltage dividers</t>
+  </si>
+  <si>
+    <t>O - I2c PU</t>
+  </si>
+  <si>
+    <t>O - Sound</t>
+  </si>
+  <si>
+    <t>O - AX Buss</t>
+  </si>
+  <si>
+    <t>* - Teensy and 5v power</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> C20</t>
+  </si>
+  <si>
+    <t>O - 3V VR</t>
+  </si>
+  <si>
+    <t>O - Arduino Shield</t>
+  </si>
+  <si>
+    <t>O - More IO pins</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>R9</t>
+  </si>
+  <si>
+    <t>O - LED</t>
+  </si>
+  <si>
+    <t>O - Button</t>
+  </si>
+  <si>
+    <t>O - Power LED</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LED</t>
+  </si>
+  <si>
+    <t>PWR</t>
+  </si>
+  <si>
+    <t>RST</t>
+  </si>
+  <si>
+    <t>BTN</t>
+  </si>
+  <si>
+    <t>O - Reset button</t>
+  </si>
+  <si>
+    <t>O - Caps for power pins</t>
+  </si>
+  <si>
+    <t>Part usage</t>
+  </si>
+  <si>
+    <t>* IO Pins and Jumpers</t>
   </si>
 </sst>
 </file>
@@ -924,7 +912,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -977,7 +965,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>17</v>
@@ -986,7 +974,7 @@
         <v>27</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>133</v>
+        <v>105</v>
       </c>
       <c r="I2" s="6">
         <v>2</v>
@@ -994,25 +982,25 @@
     </row>
     <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>137</v>
+        <v>109</v>
       </c>
       <c r="B3" s="1">
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>117</v>
+        <v>95</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>153</v>
+        <v>125</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>138</v>
+        <v>110</v>
       </c>
       <c r="I3" s="1">
         <v>2</v>
@@ -1020,13 +1008,13 @@
     </row>
     <row r="4" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>134</v>
+        <v>106</v>
       </c>
       <c r="B4" s="1">
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>117</v>
+        <v>95</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>36</v>
@@ -1038,7 +1026,7 @@
         <v>41</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>135</v>
+        <v>107</v>
       </c>
       <c r="I4" s="1">
         <v>2</v>
@@ -1072,25 +1060,25 @@
     </row>
     <row r="6" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>139</v>
+        <v>111</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>117</v>
+        <v>95</v>
       </c>
       <c r="D6" s="1">
         <v>150</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>119</v>
+        <v>97</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>140</v>
+        <v>112</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>16</v>
@@ -1101,22 +1089,22 @@
     </row>
     <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>157</v>
+        <v>129</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>159</v>
+        <v>131</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>158</v>
+        <v>130</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>8</v>
@@ -1147,13 +1135,13 @@
     </row>
     <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>154</v>
+        <v>126</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>156</v>
+        <v>128</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>14</v>
@@ -1162,7 +1150,7 @@
         <v>49</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>155</v>
+        <v>127</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>13</v>
@@ -1173,13 +1161,13 @@
     </row>
     <row r="10" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>136</v>
+        <v>108</v>
       </c>
       <c r="B10" s="1">
         <v>2</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>117</v>
+        <v>95</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>15</v>
@@ -1191,7 +1179,7 @@
         <v>41</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>136</v>
+        <v>108</v>
       </c>
       <c r="I10" s="1">
         <v>2</v>
@@ -1199,48 +1187,48 @@
     </row>
     <row r="11" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>129</v>
+        <v>101</v>
       </c>
       <c r="B11" s="1">
         <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>128</v>
+        <v>100</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>130</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>131</v>
+        <v>103</v>
       </c>
       <c r="B12" s="1">
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>128</v>
+        <v>100</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>132</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1254,7 +1242,7 @@
         <v>55</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>58</v>
@@ -1316,13 +1304,13 @@
     </row>
     <row r="17" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>143</v>
+        <v>115</v>
       </c>
       <c r="B17" s="1">
         <v>1</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>126</v>
+        <v>99</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>23</v>
@@ -1331,13 +1319,13 @@
         <v>24</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>145</v>
+        <v>117</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="I17" s="1">
         <v>3</v>
@@ -1345,13 +1333,13 @@
     </row>
     <row r="18" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>141</v>
+        <v>113</v>
       </c>
       <c r="B18" s="1">
         <v>1</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>43</v>
@@ -1363,7 +1351,7 @@
         <v>42</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>142</v>
+        <v>114</v>
       </c>
       <c r="I18" s="1">
         <v>3</v>
@@ -1371,13 +1359,13 @@
     </row>
     <row r="19" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>150</v>
+        <v>122</v>
       </c>
       <c r="B19" s="1">
         <v>1</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>152</v>
+        <v>124</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>6</v>
@@ -1386,10 +1374,10 @@
         <v>7</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>148</v>
+        <v>120</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="I19" s="1">
         <v>2</v>
@@ -1397,13 +1385,13 @@
     </row>
     <row r="20" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>147</v>
+        <v>119</v>
       </c>
       <c r="B20" s="1">
         <v>2</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>12</v>
@@ -1412,10 +1400,10 @@
         <v>74</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>148</v>
+        <v>120</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>149</v>
+        <v>121</v>
       </c>
       <c r="I20" s="1">
         <v>2</v>
@@ -1571,494 +1559,569 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD25"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="2" max="2" width="37.28515625" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
-        <v>25</v>
-      </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>139</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>140</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>140</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="1">
+        <v>2</v>
+      </c>
+      <c r="E10" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>140</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>136</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>136</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>136</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="1">
+        <v>2</v>
+      </c>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>146</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>146</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>153</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C17" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D17" s="1">
+        <v>7</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C4" t="s">
-        <v>93</v>
-      </c>
-      <c r="D4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-      <c r="F4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C5" t="s">
-        <v>97</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>134</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="6">
+        <v>2</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>145</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>145</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>141</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>147</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>147</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>152</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1</v>
+      </c>
+      <c r="E24" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>135</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D25" s="1">
+        <v>1</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>135</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1</v>
+      </c>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>135</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
-        <v>98</v>
-      </c>
-      <c r="C6" t="s">
-        <v>99</v>
-      </c>
-      <c r="E6">
-        <v>2</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>100</v>
-      </c>
-      <c r="B7" t="s">
-        <v>101</v>
-      </c>
-      <c r="C7" t="s">
-        <v>102</v>
-      </c>
-      <c r="D7" t="s">
-        <v>103</v>
-      </c>
-      <c r="E7">
-        <v>2</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>104</v>
-      </c>
-      <c r="B8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" t="s">
-        <v>105</v>
-      </c>
-      <c r="E8">
-        <v>3</v>
-      </c>
-      <c r="F8">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>71</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="C27" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D27" s="1">
+        <v>1</v>
+      </c>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>135</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D28" s="1">
+        <v>1</v>
+      </c>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>133</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C9" t="s">
-        <v>107</v>
-      </c>
-      <c r="E9">
-        <v>4</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="D29" s="1">
+        <v>2</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>133</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D30" s="1">
+        <v>2</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>155</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D31" s="1">
+        <v>2</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>155</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D32" s="1">
+        <v>2</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>155</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D33" s="1">
         <v>10</v>
       </c>
-      <c r="B10" t="s">
-        <v>108</v>
-      </c>
-      <c r="C10" t="s">
-        <v>109</v>
-      </c>
-      <c r="E10">
-        <v>6</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>72</v>
-      </c>
-      <c r="B11" t="s">
-        <v>110</v>
-      </c>
-      <c r="C11" t="s">
-        <v>111</v>
-      </c>
-      <c r="E11">
-        <v>8</v>
-      </c>
-      <c r="F11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>73</v>
-      </c>
-      <c r="B12" t="s">
-        <v>112</v>
-      </c>
-      <c r="C12" t="s">
-        <v>113</v>
-      </c>
-      <c r="E12">
-        <v>10</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>114</v>
-      </c>
-      <c r="B13" t="s">
-        <v>115</v>
-      </c>
-      <c r="C13" t="s">
-        <v>115</v>
-      </c>
-      <c r="D13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13">
-        <v>2</v>
-      </c>
-      <c r="F13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" t="s">
-        <v>116</v>
-      </c>
-      <c r="C14" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14">
-        <v>3</v>
-      </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>77</v>
-      </c>
-      <c r="B15" t="s">
-        <v>117</v>
-      </c>
-      <c r="C15" t="s">
-        <v>118</v>
-      </c>
-      <c r="D15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15">
-        <v>2</v>
-      </c>
-      <c r="F15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>78</v>
-      </c>
-      <c r="B16" t="s">
-        <v>117</v>
-      </c>
-      <c r="C16" t="s">
-        <v>118</v>
-      </c>
-      <c r="D16" t="s">
-        <v>36</v>
-      </c>
-      <c r="E16">
-        <v>2</v>
-      </c>
-      <c r="F16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>119</v>
-      </c>
-      <c r="B17" t="s">
-        <v>117</v>
-      </c>
-      <c r="C17" t="s">
-        <v>118</v>
-      </c>
-      <c r="D17">
-        <v>150</v>
-      </c>
-      <c r="E17">
-        <v>2</v>
-      </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>120</v>
-      </c>
-      <c r="B18" t="s">
-        <v>117</v>
-      </c>
-      <c r="C18" t="s">
-        <v>118</v>
-      </c>
-      <c r="D18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E18">
-        <v>2</v>
-      </c>
-      <c r="F18">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" t="s">
-        <v>117</v>
-      </c>
-      <c r="C19" t="s">
-        <v>118</v>
-      </c>
-      <c r="D19">
-        <v>330</v>
-      </c>
-      <c r="E19">
-        <v>2</v>
-      </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" t="s">
-        <v>117</v>
-      </c>
-      <c r="C20" t="s">
-        <v>118</v>
-      </c>
-      <c r="D20" t="s">
-        <v>17</v>
-      </c>
-      <c r="E20">
-        <v>2</v>
-      </c>
-      <c r="F20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" t="s">
-        <v>18</v>
-      </c>
-      <c r="E21">
-        <v>2</v>
-      </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s">
-        <v>121</v>
-      </c>
-      <c r="C22" t="s">
-        <v>13</v>
-      </c>
-      <c r="E22">
-        <v>3</v>
-      </c>
-      <c r="F22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>122</v>
-      </c>
-      <c r="B23" t="s">
-        <v>123</v>
-      </c>
-      <c r="C23" t="s">
-        <v>124</v>
-      </c>
-      <c r="E23">
-        <v>6</v>
-      </c>
-      <c r="F23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24" t="s">
-        <v>125</v>
-      </c>
-      <c r="C24" t="s">
-        <v>125</v>
-      </c>
-      <c r="E24">
-        <v>44</v>
-      </c>
-      <c r="F24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
-        <v>126</v>
-      </c>
-      <c r="C25" t="s">
-        <v>127</v>
-      </c>
-      <c r="D25" t="s">
-        <v>23</v>
-      </c>
-      <c r="E25">
-        <v>3</v>
-      </c>
-      <c r="F25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E26">
-        <v>192</v>
-      </c>
-      <c r="F26">
-        <v>69</v>
-      </c>
+      <c r="E33" s="1"/>
     </row>
   </sheetData>
+  <sortState ref="A2:J36">
+    <sortCondition ref="A2:A36"/>
+    <sortCondition ref="C2:C36"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Update to through hole version of Arduino board.
I had changes sitting that were done about a month after I fabricated
version 0.1.  I believe it had to do with beefing up ground to where the
shield picks up ground
</commit_message>
<xml_diff>
--- a/Teensy Shield Arduino Headers Through Hole/TeensyduinoTH BOM v.1.xlsx
+++ b/Teensy Shield Arduino Headers Through Hole/TeensyduinoTH BOM v.1.xlsx
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="158">
   <si>
     <t>Value</t>
   </si>
@@ -531,6 +531,12 @@
   </si>
   <si>
     <t>* IO Pins and Jumpers</t>
+  </si>
+  <si>
+    <t>WM18901-ND</t>
+  </si>
+  <si>
+    <t>Right angle version AX servo connector</t>
   </si>
 </sst>
 </file>
@@ -911,8 +917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1541,6 +1547,17 @@
       </c>
       <c r="I27" s="1">
         <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>156</v>
+      </c>
+      <c r="B28" s="1">
+        <v>0</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Reset pin has moved between Teensy 3.1 and 3.2.  Move hopefully for 3.2
Also setup size of pad/pin to hopefully use a spring loaded pin.
If directly mounting to board maybe:
http://www.digikey.com/product-detail/en/0906-0-15-20-76-14-11-0/ED8180-ND/1147048
http://www.mouser.com/ProductDetail/Mill-Max/0906-0-15-20-76-14-11-0/?qs=%2fha2pyFadug3GzwxdFHlow68khgFPrOQboHSWrH%2f7QXQhkjL7uwKMfbcxtFLmmZh
</commit_message>
<xml_diff>
--- a/Teensy Shield Arduino Headers Through Hole/TeensyduinoTH BOM v.1.xlsx
+++ b/Teensy Shield Arduino Headers Through Hole/TeensyduinoTH BOM v.1.xlsx
@@ -1,15 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kurt\Documents\GitHub\Teensy3.1-Breakout-Boards\Teensy Shield Arduino Headers Through Hole\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="14760" yWindow="-60" windowWidth="14685" windowHeight="12840"/>
   </bookViews>
   <sheets>
     <sheet name="Parts List" sheetId="1" r:id="rId1"/>
     <sheet name="Parts Usage" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="diptrace_parts_list" localSheetId="0">'Parts List'!#REF!</definedName>
@@ -62,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="161">
   <si>
     <t>Value</t>
   </si>
@@ -537,6 +541,15 @@
   </si>
   <si>
     <t>Right angle version AX servo connector</t>
+  </si>
+  <si>
+    <t>ED8180-ND</t>
+  </si>
+  <si>
+    <t>Reset - AVX spring loaded pin?</t>
+  </si>
+  <si>
+    <t>Maybe? Depends on how Teensy is mounted</t>
   </si>
 </sst>
 </file>
@@ -616,6 +629,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -671,7 +687,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -706,7 +722,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -915,10 +931,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1064,32 +1080,32 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B6" s="1">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="2">
         <v>150</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I6" s="2">
         <v>2</v>
       </c>
     </row>
@@ -1237,23 +1253,23 @@
         <v>104</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B13" s="1">
-        <v>1</v>
-      </c>
-      <c r="D13" s="1" t="s">
+      <c r="B13" s="2">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G13" s="2" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1509,26 +1525,26 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+    <row r="26" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="1">
-        <v>2</v>
-      </c>
-      <c r="C26" s="1" t="s">
+      <c r="B26" s="2">
+        <v>2</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E26" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="G26" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H26" s="1" t="s">
+      <c r="H26" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I26" s="1">
+      <c r="I26" s="2">
         <v>3</v>
       </c>
     </row>
@@ -1549,19 +1565,30 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="28" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="2">
         <v>0</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="G28" s="2" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+    <row r="29" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2141,16 +2168,4 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>